<commit_message>
Updated with 11 AM April 6 data.  Added explanation text boxes to charts.
</commit_message>
<xml_diff>
--- a/SARS-CoV-2 Infection Odds - Miami Beach.xlsx
+++ b/SARS-CoV-2 Infection Odds - Miami Beach.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/work/Library/Mobile Documents/com~apple~CloudDocs/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C030278F-10DC-9845-97D7-6E4FC015A14A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6E710B-D369-844F-86CF-A6DAF7E78795}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{5746141D-E7E8-714E-A98D-1CE69C8603B7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{5746141D-E7E8-714E-A98D-1CE69C8603B7}"/>
   </bookViews>
   <sheets>
     <sheet name="number of infections" sheetId="3" r:id="rId1"/>
@@ -18,51 +18,7 @@
     <sheet name="infection odds" sheetId="2" r:id="rId3"/>
     <sheet name="data" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">data!$A$2:$A$15</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">data!$K$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">data!$L$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">data!$L$2:$L$15</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">data!$M$1</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">data!$M$2:$M$15</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">data!$A$2:$A$15</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">data!$K$1</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">data!$K$2:$K$15</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">data!$L$1</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">data!$L$2:$L$15</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">data!$M$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">data!$K$2:$K$15</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">data!$M$2:$M$15</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">data!$A$2:$A$15</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">data!$K$1</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">data!$K$2:$K$15</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">data!$L$1</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">data!$L$2:$L$15</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">data!$M$1</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">data!$M$2:$M$15</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">data!$A$2:$A$15</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">data!$K$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">data!$L$1</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">data!$K$2:$K$15</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">data!$L$1</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">data!$L$2:$L$15</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">data!$M$1</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">data!$M$2:$M$15</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">data!$A$2:$A$15</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">data!$K$1</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">data!$K$2:$K$15</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">data!$L$1</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">data!$L$2:$L$15</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">data!$L$2:$L$15</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">data!$M$1</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">data!$M$2:$M$15</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">data!$N$1</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">data!$N$2:$N$15</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">data!$A$2:$A$15</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">data!$K$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">data!$K$2:$K$15</definedName>
-  </definedNames>
-  <calcPr calcId="181029" refMode="R1C1"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -271,6 +227,100 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
@@ -347,45 +397,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Helvetica"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Helvetica"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -405,80 +417,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Helvetica"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Helvetica"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Helvetica"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Helvetica"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <font>
@@ -554,6 +492,24 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -694,10 +650,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>data!$A$2:$A$15</c:f>
+              <c:f>data!$A$2:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>43913</c:v>
                 </c:pt>
@@ -739,16 +695,19 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>43926</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43927</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$C$2:$C$15</c:f>
+              <c:f>data!$C$2:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>165</c:v>
                 </c:pt>
@@ -790,6 +749,9 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1825</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1915</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -826,10 +788,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>data!$A$2:$A$15</c:f>
+              <c:f>data!$A$2:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>43913</c:v>
                 </c:pt>
@@ -871,16 +833,19 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>43926</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43927</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$E$2:$E$15</c:f>
+              <c:f>data!$E$2:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>66</c:v>
                 </c:pt>
@@ -922,6 +887,9 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>766</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1096,8 +1064,8 @@
               <c:idx val="13"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.6949152542372881E-3"/>
-                  <c:y val="-2.7118644067796641E-2"/>
+                  <c:x val="-1.6949152542374123E-3"/>
+                  <c:y val="-6.2146174737453527E-17"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1110,6 +1078,27 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-748D-CB43-A627-A86316C7767B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-2.2033898305084808E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-710F-4244-96A2-807873A8045E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1222,10 +1211,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$F$2:$F$15</c:f>
+              <c:f>data!$F$2:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>198</c:v>
                 </c:pt>
@@ -1267,6 +1256,9 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>2190</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2298</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1446,6 +1438,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -1554,10 +1547,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>data!$A$2:$A$15</c:f>
+              <c:f>data!$A$2:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>43913</c:v>
                 </c:pt>
@@ -1599,16 +1592,19 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>43926</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43927</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$G$2:$G$15</c:f>
+              <c:f>data!$G$2:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1.7875134063505477E-3</c:v>
                 </c:pt>
@@ -1650,6 +1646,9 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1.9770981615695449E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.0745988928250296E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1686,10 +1685,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>data!$A$2:$A$15</c:f>
+              <c:f>data!$A$2:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>43913</c:v>
                 </c:pt>
@@ -1731,16 +1730,19 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>43926</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43927</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$I$2:$I$15</c:f>
+              <c:f>data!$I$2:$I$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>7.1500536254021888E-4</c:v>
                 </c:pt>
@@ -1782,6 +1784,9 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>7.9083926462781805E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.2983955713001184E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1978,7 +1983,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="0"/>
-                  <c:y val="-2.3728813559322035E-2"/>
+                  <c:y val="5.0847457627118025E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1991,6 +1996,27 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000007-E7E6-984F-B4E4-5660F27577B3}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-2.5423728813559324E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-AF72-1848-8D14-2279B6F7C74F}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2052,10 +2078,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>data!$A$2:$A$15</c:f>
+              <c:f>data!$A$2:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>43913</c:v>
                 </c:pt>
@@ -2097,16 +2123,19 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>43926</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43927</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$J$2:$J$15</c:f>
+              <c:f>data!$J$2:$J$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>2.1450160876206573E-3</c:v>
                 </c:pt>
@@ -2148,6 +2177,9 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>2.3725177938834538E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.4895186713900355E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2327,6 +2359,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -2441,10 +2474,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>data!$A$2:$A$15</c:f>
+              <c:f>data!$A$2:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>43913</c:v>
                 </c:pt>
@@ -2486,16 +2519,19 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>43926</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43927</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$L$2:$L$15</c:f>
+              <c:f>data!$L$2:$L$16</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>399.59740259740261</c:v>
                 </c:pt>
@@ -2537,6 +2573,9 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>36.1279843444227</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>34.430063409175681</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2573,10 +2612,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>data!$A$2:$A$15</c:f>
+              <c:f>data!$A$2:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>43913</c:v>
                 </c:pt>
@@ -2618,16 +2657,19 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>43926</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43927</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$M$2:$M$15</c:f>
+              <c:f>data!$M$2:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>159.83896103896097</c:v>
                 </c:pt>
@@ -2669,6 +2711,9 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>14.451193737769081</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13.772025363670274</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2792,10 +2837,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>data!$A$2:$A$15</c:f>
+              <c:f>data!$A$2:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>43913</c:v>
                 </c:pt>
@@ -2837,16 +2882,19 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>43926</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43927</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$N$2:$N$15</c:f>
+              <c:f>data!$N$2:$N$16</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>479.51688311688309</c:v>
                 </c:pt>
@@ -2888,6 +2936,9 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>43.353581213307237</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41.316076091010814</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3067,6 +3118,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -4727,6 +4779,9 @@
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CE3B9B0-3433-2A43-A939-51D78C203FCD}"/>
             </a:ext>
+            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="0"/>
+            </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
@@ -4749,6 +4804,183 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.44746</cdr:x>
+      <cdr:y>0.92542</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>1</cdr:x>
+      <cdr:y>0.95424</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{879F44A7-087F-AD4F-A3B0-AC4862A1AEFD}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3352800" y="6934200"/>
+          <a:ext cx="4140200" cy="215900"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>source: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
+              <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id=""/>
+            </a:rPr>
+            <a:t>https://www.floridadisaster.org/news-media/news/</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.13898</cdr:x>
+      <cdr:y>0.12203</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.61864</cdr:x>
+      <cdr:y>0.31525</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FACEC6B-C4C5-3E47-91AE-E9058A2F8EE6}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1041400" y="914400"/>
+          <a:ext cx="3594100" cy="1447800"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.11017</cdr:x>
+      <cdr:y>0.25763</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.52373</cdr:x>
+      <cdr:y>0.35254</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCC04FA3-4C1D-104C-9CF8-D4910BADB4DA}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="825500" y="1930400"/>
+          <a:ext cx="3098800" cy="711200"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1600">
+              <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
+            </a:rPr>
+            <a:t>The bars</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
+            </a:rPr>
+            <a:t> illustrate the range of possible infections, from 5x to 7x the confirmed case count.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1600">
+            <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4791,7 +5023,227 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.44746</cdr:x>
+      <cdr:y>0.92542</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>1</cdr:x>
+      <cdr:y>0.95424</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{381B6C67-ABC4-EC4D-BA80-680BA1D6535C}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3352800" y="6934200"/>
+          <a:ext cx="4140200" cy="215900"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>source: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
+              <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id=""/>
+            </a:rPr>
+            <a:t>https://www.floridadisaster.org/news-media/news/</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.12542</cdr:x>
+      <cdr:y>0.21864</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.77797</cdr:x>
+      <cdr:y>0.31356</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6F50128-A32A-3744-B700-B421E24B7189}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="939800" y="1638300"/>
+          <a:ext cx="4889500" cy="711200"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600">
+              <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
+            </a:rPr>
+            <a:t>The bars</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
+            </a:rPr>
+            <a:t> illustrate the range of possible infection percentages, as the range of infection counts varies from 5x to 7x the confirmed case count.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1600">
+            <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4831,10 +5283,234 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{381B6C67-ABC4-EC4D-BA80-680BA1D6535C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="495300" y="6972300"/>
+          <a:ext cx="4140200" cy="215900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0"/>
+        <a:lstStyle>
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>source: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
+            </a:rPr>
+            <a:t>https://www.floridadisaster.org/news-media/news/</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.29153</cdr:x>
+      <cdr:y>0.11017</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>1</cdr:x>
+      <cdr:y>0.21186</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04C86D55-AD5D-0647-BDF9-E042E5833A90}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2184400" y="825500"/>
+          <a:ext cx="5308600" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600">
+              <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
+            </a:rPr>
+            <a:t>The bars</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
+            </a:rPr>
+            <a:t> illustrate the range of possible odds of a single person having been infected, as the range of infection counts varies from 5x to 7x the confirmed case count.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1600">
+            <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -5060,7 +5736,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Mathematical modelers in the Centre for the Mathematical Modelling of Infectious Diseases at the London School of Hygiene &amp; Tropical Medicine found the U.S.’s case count likely represented just 14% to 19% of actual infections, so multiply the number of cases by five.</a:t>
+            <a:t>Mathematical modelers in the Centre for the Mathematical Modelling of Infectious Diseases at the London School of Hygiene &amp; Tropical Medicine found the U.S.’s case count likely represented just 14% to 19% of actual infections, so multiply the number of cases by five to seven.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -5078,53 +5754,49 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BE4AE7D-0714-C143-A688-292634C906F9}" name="Table2" displayName="Table2" ref="A1:O18" totalsRowShown="0" headerRowDxfId="16" dataDxfId="10" headerRowCellStyle="Heading 3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3BE4AE7D-0714-C143-A688-292634C906F9}" name="Table2" displayName="Table2" ref="A1:O18" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" headerRowCellStyle="Heading 3">
   <autoFilter ref="A1:O18" xr:uid="{550F0C45-D7F8-B94B-924D-6E337BF889A7}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{5A8F4760-7ADB-5643-B32D-8C30EC7E1E18}" name="date" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{1A056131-5760-2749-834E-BF55DAB2649A}" name="cases" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{C899EFA6-17F8-B447-A1DB-6D7083A2F531}" name="infection count estimating 5x cases infected" dataDxfId="13">
+    <tableColumn id="1" xr3:uid="{5A8F4760-7ADB-5643-B32D-8C30EC7E1E18}" name="date" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{1A056131-5760-2749-834E-BF55DAB2649A}" name="cases" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{C899EFA6-17F8-B447-A1DB-6D7083A2F531}" name="infection count estimating 5x cases infected" dataDxfId="12">
       <calculatedColumnFormula>Table2[[#This Row],[cases]]*5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{9DA1C9E0-36F7-DE43-8448-4D8CE8B57839}" name="infection count, estimating 7x cases infected" dataDxfId="12">
+    <tableColumn id="9" xr3:uid="{9DA1C9E0-36F7-DE43-8448-4D8CE8B57839}" name="infection count, estimating 7x cases infected" dataDxfId="11">
       <calculatedColumnFormula>Table2[[#This Row],[cases]]*7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{DF5E18EF-399D-9948-A8F2-9862C2232353}" name="infection count difference" dataDxfId="9">
+    <tableColumn id="11" xr3:uid="{DF5E18EF-399D-9948-A8F2-9862C2232353}" name="infection count difference" dataDxfId="10">
       <calculatedColumnFormula>Table2[[#This Row],[infection count, estimating 7x cases infected]]-Table2[[#This Row],[infection count estimating 5x cases infected]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{F5EF272D-BCCD-9A42-A437-406EF6A3644D}" name="average infection count" dataDxfId="7">
+    <tableColumn id="10" xr3:uid="{F5EF272D-BCCD-9A42-A437-406EF6A3644D}" name="average infection count" dataDxfId="9">
       <calculatedColumnFormula>(Table2[[#This Row],[infection count estimating 5x cases infected]]+Table2[[#This Row],[infection count, estimating 7x cases infected]])/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{8AB0CE19-F28B-1B41-B08C-6F528E4C628D}" name="infection percentage, estimating 5x cases infected" dataDxfId="3">
+    <tableColumn id="12" xr3:uid="{8AB0CE19-F28B-1B41-B08C-6F528E4C628D}" name="infection percentage, estimating 5x cases infected" dataDxfId="8">
       <calculatedColumnFormula>Table2[[#This Row],[infection count estimating 5x cases infected]]/$O$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{1109EB50-6E0E-5D49-923A-162321C9390D}" name="infection percentage, estimating 7x cases infected" dataDxfId="2">
+    <tableColumn id="13" xr3:uid="{1109EB50-6E0E-5D49-923A-162321C9390D}" name="infection percentage, estimating 7x cases infected" dataDxfId="7">
       <calculatedColumnFormula>Table2[[#This Row],[infection count, estimating 7x cases infected]]/$O$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{238DA9D3-166B-A04A-B1CF-89D64E5C9BCE}" name="infection percentage difference" dataDxfId="1">
+    <tableColumn id="14" xr3:uid="{238DA9D3-166B-A04A-B1CF-89D64E5C9BCE}" name="infection percentage difference" dataDxfId="6">
       <calculatedColumnFormula>Table2[[#This Row],[infection percentage, estimating 7x cases infected]]-Table2[[#This Row],[infection percentage, estimating 5x cases infected]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{DE45558E-71C3-0C4E-A3A2-8B967C3E17AB}" name="average infection percentage" dataDxfId="0">
+    <tableColumn id="15" xr3:uid="{DE45558E-71C3-0C4E-A3A2-8B967C3E17AB}" name="average infection percentage" dataDxfId="5">
       <calculatedColumnFormula>(Table2[[#This Row],[infection percentage, estimating 5x cases infected]]+Table2[[#This Row],[infection percentage, estimating 7x cases infected]])/2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{02005BA0-C3BB-F54B-908A-B7ECE76A73E8}" name="1-in-X odds, estimating 5x cases infected" dataDxfId="4">
       <calculatedColumnFormula>$O$3/(Table2[[#This Row],[cases]]*5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{244EEAB7-EA2F-9142-A896-C40C6D4A9BE9}" name="1-in-X odds, estimating 7x cases infected" dataDxfId="6">
+    <tableColumn id="4" xr3:uid="{244EEAB7-EA2F-9142-A896-C40C6D4A9BE9}" name="1-in-X odds, estimating 7x cases infected" dataDxfId="3">
       <calculatedColumnFormula>$O$3/(Table2[[#This Row],[cases]]*7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8F986CA1-2145-0B4C-AAAE-6153D0E4F495}" name="1-in-X odds difference" dataDxfId="5">
+    <tableColumn id="5" xr3:uid="{8F986CA1-2145-0B4C-AAAE-6153D0E4F495}" name="1-in-X odds difference" dataDxfId="2">
       <calculatedColumnFormula>Table2[[#This Row],[1-in-X odds, estimating 5x cases infected]]-Table2[[#This Row],[1-in-X odds, estimating 7x cases infected]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A840ABA5-36ED-FF4A-9BD9-42132A34A0D4}" name="average 1-in-X odds" dataDxfId="11">
+    <tableColumn id="6" xr3:uid="{A840ABA5-36ED-FF4A-9BD9-42132A34A0D4}" name="average 1-in-X odds" dataDxfId="1">
       <calculatedColumnFormula>(Table2[[#This Row],[1-in-X odds, estimating 5x cases infected]]+Table2[[#This Row],[1-in-X odds, estimating 7x cases infected]])/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{3F9CC5ED-74BF-8D4B-A8C4-40AA15D26E71}" name="constants" dataDxfId="8"/>
+    <tableColumn id="16" xr3:uid="{3F9CC5ED-74BF-8D4B-A8C4-40AA15D26E71}" name="constants" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5429,13 +6101,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD26BEB-40E2-ED4B-A542-5EA1102CBE4A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -5444,8 +6117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CBF10BE-52FE-794B-890A-D6D4B91A185A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5460,7 +6133,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5474,8 +6147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E1E0E18-E130-924E-B8A9-7F036230CE4B}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6350,54 +7023,56 @@
       <c r="A16" s="9">
         <v>43927</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="10">
+        <v>383</v>
+      </c>
       <c r="C16" s="1">
         <f>Table2[[#This Row],[cases]]*5</f>
-        <v>0</v>
+        <v>1915</v>
       </c>
       <c r="D16" s="1">
         <f>Table2[[#This Row],[cases]]*7</f>
-        <v>0</v>
+        <v>2681</v>
       </c>
       <c r="E16" s="1">
         <f>Table2[[#This Row],[infection count, estimating 7x cases infected]]-Table2[[#This Row],[infection count estimating 5x cases infected]]</f>
-        <v>0</v>
+        <v>766</v>
       </c>
       <c r="F16" s="1">
         <f>(Table2[[#This Row],[infection count estimating 5x cases infected]]+Table2[[#This Row],[infection count, estimating 7x cases infected]])/2</f>
-        <v>0</v>
+        <v>2298</v>
       </c>
       <c r="G16" s="16">
         <f>Table2[[#This Row],[infection count estimating 5x cases infected]]/$O$3</f>
-        <v>0</v>
+        <v>2.0745988928250296E-2</v>
       </c>
       <c r="H16" s="15">
         <f>Table2[[#This Row],[infection count, estimating 7x cases infected]]/$O$3</f>
-        <v>0</v>
+        <v>2.9044384499550414E-2</v>
       </c>
       <c r="I16" s="16">
         <f>Table2[[#This Row],[infection percentage, estimating 7x cases infected]]-Table2[[#This Row],[infection percentage, estimating 5x cases infected]]</f>
-        <v>0</v>
+        <v>8.2983955713001184E-3</v>
       </c>
       <c r="J16" s="16">
         <f>(Table2[[#This Row],[infection percentage, estimating 5x cases infected]]+Table2[[#This Row],[infection percentage, estimating 7x cases infected]])/2</f>
-        <v>0</v>
-      </c>
-      <c r="K16" s="3" t="e">
+        <v>2.4895186713900355E-2</v>
+      </c>
+      <c r="K16" s="3">
         <f>$O$3/(Table2[[#This Row],[cases]]*5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L16" s="3" t="e">
+        <v>48.202088772845954</v>
+      </c>
+      <c r="L16" s="3">
         <f>$O$3/(Table2[[#This Row],[cases]]*7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M16" s="3" t="e">
+        <v>34.430063409175681</v>
+      </c>
+      <c r="M16" s="3">
         <f>Table2[[#This Row],[1-in-X odds, estimating 5x cases infected]]-Table2[[#This Row],[1-in-X odds, estimating 7x cases infected]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N16" s="3" t="e">
+        <v>13.772025363670274</v>
+      </c>
+      <c r="N16" s="3">
         <f>(Table2[[#This Row],[1-in-X odds, estimating 5x cases infected]]+Table2[[#This Row],[1-in-X odds, estimating 7x cases infected]])/2</f>
-        <v>#DIV/0!</v>
+        <v>41.316076091010814</v>
       </c>
       <c r="O16" s="3"/>
     </row>

</xml_diff>